<commit_message>
feat : generate items rest api
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\auto_catalog_create\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DE8F03-0221-4B93-9285-3122AB4AE48F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE86165-27CD-41BA-B217-B36641F071FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>cat1</t>
   </si>
@@ -40,64 +40,16 @@
     <t>Reembolso</t>
   </si>
   <si>
-    <t>Compra de Passagem</t>
-  </si>
-  <si>
-    <t>Sala de Reunião</t>
-  </si>
-  <si>
-    <t>serviços</t>
-  </si>
-  <si>
-    <t>timecard</t>
-  </si>
-  <si>
-    <t>Banco de Horas</t>
-  </si>
-  <si>
-    <t>Recursos Humanos</t>
-  </si>
-  <si>
-    <t>Férias</t>
-  </si>
-  <si>
-    <t>Treinamento</t>
-  </si>
-  <si>
-    <t>Certificação</t>
-  </si>
-  <si>
-    <t>Solicitar Certificação</t>
-  </si>
-  <si>
-    <t>Cadastrar novo</t>
-  </si>
-  <si>
-    <t>curso</t>
-  </si>
-  <si>
-    <t>Aliancas</t>
-  </si>
-  <si>
-    <t>Parceiros</t>
-  </si>
-  <si>
-    <t>Cadastrar</t>
+    <t>recursos humanos</t>
   </si>
   <si>
     <t>teste</t>
   </si>
   <si>
-    <t>serv1</t>
-  </si>
-  <si>
-    <t>serv3</t>
-  </si>
-  <si>
-    <t>cert1</t>
-  </si>
-  <si>
-    <t>cada2</t>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>item1</t>
   </si>
 </sst>
 </file>
@@ -402,10 +354,13 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -434,104 +389,59 @@
     </row>
     <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A7" s="5"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="5"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>